<commit_message>
Modelo por BIC seleccionado, incorporada comparación por BIC, análisis de regresión incluidos (grado 2 - motor 1; grado 9 - motor 2)
</commit_message>
<xml_diff>
--- a/data/RESULTADOS(EnConstr).xlsx
+++ b/data/RESULTADOS(EnConstr).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BETA\Desktop\pruebas_programas\Proyecto_probabilidad\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{587D8749-0574-40D0-A41C-3D7F198EE34D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C380F97-AAC0-42BF-8B21-407A87E42FBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>n</t>
   </si>
@@ -62,13 +62,17 @@
   <si>
     <t>Motor 2</t>
   </si>
+  <si>
+    <t>BIC</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -111,7 +115,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -149,15 +153,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -171,17 +166,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -212,25 +196,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -253,19 +224,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -274,28 +245,37 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -510,6 +490,56 @@
         <a:xfrm>
           <a:off x="5848350" y="114300"/>
           <a:ext cx="342857" cy="180952"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>600004</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>238102</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagen 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3223DAE-BD7A-443D-8746-D58AE0826DFC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2095500" y="2905125"/>
+          <a:ext cx="571429" cy="180952"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -784,23 +814,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="19.5" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.140625" style="1" customWidth="1"/>
-    <col min="3" max="6" width="9.140625" style="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="11.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
     <col min="7" max="7" width="10.85546875" style="2" customWidth="1"/>
     <col min="8" max="8" width="12" style="3" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="9.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
@@ -820,42 +854,42 @@
       <c r="G1" s="18"/>
       <c r="H1" s="19"/>
       <c r="I1" s="20"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J1"/>
+    </row>
+    <row r="2" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="21">
+        <v>2</v>
+      </c>
+      <c r="D2" s="21">
+        <v>1000</v>
+      </c>
+      <c r="E2" s="21">
+        <v>0</v>
+      </c>
+      <c r="F2" s="21">
+        <v>18</v>
+      </c>
+      <c r="G2" s="25">
+        <v>1027.6199999999999</v>
+      </c>
+      <c r="H2" s="13">
+        <v>10.0775097024299</v>
+      </c>
+      <c r="I2" s="7">
+        <f>(H2)/9.80665</f>
+        <v>1.0276200030010147</v>
+      </c>
+      <c r="J2"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="C3" s="7">
         <v>6</v>
-      </c>
-      <c r="D2" s="7">
-        <v>1000</v>
-      </c>
-      <c r="E2" s="7">
-        <v>0</v>
-      </c>
-      <c r="F2" s="7">
-        <v>18</v>
-      </c>
-      <c r="G2" s="11">
-        <v>1096.699738</v>
-      </c>
-      <c r="H2" s="14">
-        <v>10.754950486</v>
-      </c>
-      <c r="I2" s="21">
-        <f>(H2)/9.80665</f>
-        <v>1.0966997380349051</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7"/>
-      <c r="C3" s="7">
-        <v>8</v>
       </c>
       <c r="D3" s="7">
         <v>1000</v>
@@ -867,23 +901,22 @@
         <v>18</v>
       </c>
       <c r="G3" s="11">
-        <v>1840.847491</v>
+        <v>1096.699738</v>
       </c>
       <c r="H3" s="14">
-        <v>18.052547048000001</v>
-      </c>
-      <c r="I3" s="21">
-        <f t="shared" ref="I3:I9" si="0">(H3)/9.80665</f>
-        <v>1.8408474910392441</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+        <v>10.754950486</v>
+      </c>
+      <c r="I3" s="7">
+        <f>(H3)/9.80665</f>
+        <v>1.0966997380349051</v>
+      </c>
+      <c r="J3"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="6"/>
-      <c r="B4" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="B4" s="7"/>
       <c r="C4" s="7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D4" s="7">
         <v>1000</v>
@@ -892,108 +925,112 @@
         <v>0</v>
       </c>
       <c r="F4" s="7">
+        <v>18</v>
+      </c>
+      <c r="G4" s="11">
+        <v>1840.847491</v>
+      </c>
+      <c r="H4" s="14">
+        <v>18.052547048000001</v>
+      </c>
+      <c r="I4" s="7">
+        <f t="shared" ref="I4:I11" si="0">(H4)/9.80665</f>
+        <v>1.8408474910392441</v>
+      </c>
+      <c r="J4"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="7">
+        <v>6</v>
+      </c>
+      <c r="D5" s="7">
+        <v>1000</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7">
         <v>60</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G5" s="11">
         <v>3225.7371429999998</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H5" s="13">
         <v>31.633675245782499</v>
       </c>
-      <c r="I4" s="21">
+      <c r="I5" s="7">
         <f t="shared" si="0"/>
         <v>3.2257371524202965</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9">
+      <c r="J5"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9">
         <v>8</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D6" s="9">
         <v>1000</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E6" s="9">
         <v>0</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F6" s="9">
         <v>60</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G6" s="12">
         <v>5885.677713</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H6" s="15">
         <v>57.718781512750702</v>
       </c>
-      <c r="I5" s="22">
+      <c r="I6" s="9">
         <f t="shared" si="0"/>
         <v>5.8856777301882603</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A6" s="4" t="s">
+      <c r="J6"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C7" s="5">
         <v>6</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D7" s="5">
         <v>1000</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E7" s="5">
         <v>0</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F7" s="5">
         <v>18</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G7" s="10">
         <v>1161.2343499999999</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H7" s="13">
         <v>11.3878188716839</v>
       </c>
-      <c r="I6" s="21">
+      <c r="I7" s="7">
         <f t="shared" si="0"/>
         <v>1.1612343533912091</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7">
+      <c r="J7"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A8" s="6"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7">
         <v>8</v>
-      </c>
-      <c r="D7" s="7">
-        <v>1000</v>
-      </c>
-      <c r="E7" s="7">
-        <v>0</v>
-      </c>
-      <c r="F7" s="7">
-        <v>18</v>
-      </c>
-      <c r="G7" s="11">
-        <v>5479.4858640000002</v>
-      </c>
-      <c r="H7" s="13">
-        <v>53.735400205121998</v>
-      </c>
-      <c r="I7" s="21">
-        <f>(H7)/9.80665</f>
-        <v>5.4794858800020396</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="7">
-        <v>6</v>
       </c>
       <c r="D8" s="7">
         <v>1000</v>
@@ -1002,44 +1039,305 @@
         <v>0</v>
       </c>
       <c r="F8" s="7">
+        <v>18</v>
+      </c>
+      <c r="G8" s="11">
+        <v>5479.4858640000002</v>
+      </c>
+      <c r="H8" s="13">
+        <v>53.735400205121998</v>
+      </c>
+      <c r="I8" s="7">
+        <f>(H8)/9.80665</f>
+        <v>5.4794858800020396</v>
+      </c>
+      <c r="J8"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="C9" s="1">
+        <v>9</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>18</v>
+      </c>
+      <c r="G9" s="2">
+        <v>3366.8949149</v>
+      </c>
+      <c r="H9" s="3">
+        <v>33.017960113628199</v>
+      </c>
+      <c r="I9" s="7">
+        <f>(H9)/9.80665</f>
+        <v>3.3668949247325233</v>
+      </c>
+      <c r="J9"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A10" s="6"/>
+      <c r="B10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="7">
+        <v>6</v>
+      </c>
+      <c r="D10" s="7">
+        <v>1000</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0</v>
+      </c>
+      <c r="F10" s="7">
         <v>51</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G10" s="11">
         <v>1538.2724679999999</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H10" s="13">
         <v>15.085299742366599</v>
       </c>
-      <c r="I8" s="21">
+      <c r="I10" s="7">
         <f t="shared" si="0"/>
         <v>1.5382724724922987</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A9" s="8"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="9">
+      <c r="J10"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9"/>
+      <c r="C11" s="9">
         <v>8</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D11" s="9">
         <v>1000</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E11" s="9">
         <v>0</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F11" s="9">
         <v>51</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G11" s="12">
         <v>2987.1871970000002</v>
       </c>
-      <c r="H9" s="15">
+      <c r="H11" s="15">
         <v>29.294299411009799</v>
       </c>
-      <c r="I9" s="22">
+      <c r="I11" s="9">
         <f t="shared" si="0"/>
         <v>2.9871872057236466</v>
       </c>
+      <c r="J11"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A14" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="D15" s="23">
+        <v>227.80446621658101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A16" s="6"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="1">
+        <v>3</v>
+      </c>
+      <c r="D16" s="23">
+        <v>228.28957330231</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C17" s="1">
+        <v>4</v>
+      </c>
+      <c r="D17" s="23">
+        <v>230.609661273131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="1">
+        <v>5</v>
+      </c>
+      <c r="D18" s="23">
+        <v>233.40289394959899</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C19" s="1">
+        <v>6</v>
+      </c>
+      <c r="D19" s="23">
+        <v>236.29012455883699</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="1">
+        <v>7</v>
+      </c>
+      <c r="D20" s="23">
+        <v>238.77914876086999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A21" s="6"/>
+      <c r="C21" s="1">
+        <v>8</v>
+      </c>
+      <c r="D21" s="23">
+        <v>241.09262398007101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="1">
+        <v>9</v>
+      </c>
+      <c r="D22" s="23">
+        <v>243.69190736543001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C23" s="1">
+        <v>10</v>
+      </c>
+      <c r="D23" s="23">
+        <v>244.12634223964599</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A24" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="5">
+        <v>2</v>
+      </c>
+      <c r="D24" s="24">
+        <v>145.01604173568299</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C25" s="1">
+        <v>3</v>
+      </c>
+      <c r="D25" s="23">
+        <v>147.53456132436099</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C26" s="1">
+        <v>4</v>
+      </c>
+      <c r="D26" s="23">
+        <v>142.26463600282301</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C27" s="1">
+        <v>5</v>
+      </c>
+      <c r="D27" s="23">
+        <v>141.66938060444201</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C28" s="1">
+        <v>6</v>
+      </c>
+      <c r="D28" s="23">
+        <v>137.71428667469499</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C29" s="1">
+        <v>7</v>
+      </c>
+      <c r="D29" s="23">
+        <v>137.406592278087</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C30" s="1">
+        <v>8</v>
+      </c>
+      <c r="D30" s="23">
+        <v>130.62023564650701</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C31" s="1">
+        <v>9</v>
+      </c>
+      <c r="D31" s="23">
+        <v>125.47820283448399</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C32" s="1">
+        <v>10</v>
+      </c>
+      <c r="D32" s="23">
+        <v>126.77055148453</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="B33" s="7"/>
+      <c r="D33" s="23"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="D34" s="23"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="D35" s="23"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="D36" s="23"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="D37" s="23"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="D38" s="23"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="D39" s="23"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="D40" s="23"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.4">
+      <c r="D41" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>